<commit_message>
Added Update Test and Create Test and committed excel file with the test Results
</commit_message>
<xml_diff>
--- a/Project 4/Connected Office Test Data.xlsx
+++ b/Project 4/Connected Office Test Data.xlsx
@@ -1204,14 +1204,14 @@
       <x:c r="A2" s="2" t="s">
         <x:v>41</x:v>
       </x:c>
-      <x:c r="B2" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="B2" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C2" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="D2" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="D2" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="E2" s="2" t="s">
         <x:v>75</x:v>
@@ -1221,14 +1221,14 @@
       <x:c r="A3" s="2" t="s">
         <x:v>43</x:v>
       </x:c>
-      <x:c r="B3" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="B3" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C3" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="D3" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="D3" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="E3" s="2" t="s">
         <x:v>75</x:v>
@@ -1238,14 +1238,14 @@
       <x:c r="A4" s="2" t="s">
         <x:v>45</x:v>
       </x:c>
-      <x:c r="B4" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="B4" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C4" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="D4" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="D4" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="E4" s="2" t="s">
         <x:v>75</x:v>
@@ -1255,14 +1255,14 @@
       <x:c r="A5" s="2" t="s">
         <x:v>47</x:v>
       </x:c>
-      <x:c r="B5" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="B5" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C5" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="D5" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="D5" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="E5" s="2" t="s">
         <x:v>75</x:v>
@@ -1272,14 +1272,14 @@
       <x:c r="A6" s="2" t="s">
         <x:v>49</x:v>
       </x:c>
-      <x:c r="B6" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="B6" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C6" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="D6" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="D6" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="E6" s="2" t="s">
         <x:v>75</x:v>
@@ -1289,14 +1289,14 @@
       <x:c r="A7" s="2" t="s">
         <x:v>52</x:v>
       </x:c>
-      <x:c r="B7" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="B7" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C7" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="D7" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="D7" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="E7" s="2" t="s">
         <x:v>75</x:v>
@@ -1306,14 +1306,14 @@
       <x:c r="A8" s="2" t="s">
         <x:v>54</x:v>
       </x:c>
-      <x:c r="B8" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="B8" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C8" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="D8" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="D8" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="E8" s="2" t="s">
         <x:v>75</x:v>
@@ -1323,14 +1323,14 @@
       <x:c r="A9" s="2" t="s">
         <x:v>56</x:v>
       </x:c>
-      <x:c r="B9" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="B9" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C9" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="D9" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="D9" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="E9" s="2" t="s">
         <x:v>75</x:v>
@@ -1340,14 +1340,14 @@
       <x:c r="A10" s="2" t="s">
         <x:v>58</x:v>
       </x:c>
-      <x:c r="B10" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="B10" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C10" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="D10" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="D10" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="E10" s="2" t="s">
         <x:v>75</x:v>
@@ -1357,14 +1357,14 @@
       <x:c r="A11" s="2" t="s">
         <x:v>61</x:v>
       </x:c>
-      <x:c r="B11" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="B11" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C11" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="D11" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="D11" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="E11" s="2" t="s">
         <x:v>75</x:v>
@@ -1374,14 +1374,14 @@
       <x:c r="A12" s="2" t="s">
         <x:v>63</x:v>
       </x:c>
-      <x:c r="B12" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="B12" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C12" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="D12" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="D12" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="E12" s="2" t="s">
         <x:v>75</x:v>
@@ -1391,14 +1391,14 @@
       <x:c r="A13" s="2" t="s">
         <x:v>65</x:v>
       </x:c>
-      <x:c r="B13" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="B13" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C13" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="D13" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="D13" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="E13" s="2" t="s">
         <x:v>75</x:v>
@@ -1408,14 +1408,14 @@
       <x:c r="A14" s="2" t="s">
         <x:v>67</x:v>
       </x:c>
-      <x:c r="B14" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="B14" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C14" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="D14" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="D14" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="E14" s="2" t="s">
         <x:v>75</x:v>
@@ -1425,14 +1425,14 @@
       <x:c r="A15" s="2" t="s">
         <x:v>69</x:v>
       </x:c>
-      <x:c r="B15" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="B15" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C15" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="D15" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="D15" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="E15" s="2" t="s">
         <x:v>75</x:v>
@@ -1442,153 +1442,158 @@
       <x:c r="A16" s="2" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="B16" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="B16" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C16" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="D16" s="2" t="b">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E16" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="D16" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="E16" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A17" s="2" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="B17" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="B17" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C17" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="D17" s="2" t="b">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E17" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="D17" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="E17" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A18" s="2" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="B18" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="B18" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C18" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="D18" s="2" t="b">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E18" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="D18" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="E18" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A19" s="2" t="s">
         <x:v>20</x:v>
       </x:c>
-      <x:c r="B19" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="B19" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C19" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="D19" s="2" t="b">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E19" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="D19" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="E19" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A20" s="2" t="s">
         <x:v>24</x:v>
       </x:c>
-      <x:c r="B20" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="B20" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C20" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="D20" s="2" t="b">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E20" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="D20" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="E20" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A21" s="2" t="s">
         <x:v>27</x:v>
       </x:c>
-      <x:c r="B21" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="B21" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C21" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="D21" s="2" t="b">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E21" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="D21" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="E21" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A22" s="2" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="B22" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="B22" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C22" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="D22" s="2" t="b">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E22" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="D22" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="E22" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A23" s="2" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="B23" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="B23" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C23" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="D23" s="2" t="b">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E23" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="D23" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="E23" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A24" s="2" t="s">
         <x:v>37</x:v>
       </x:c>
-      <x:c r="B24" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="B24" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C24" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="D24" s="2" t="b">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E24" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="D24" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="E24" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:5">
+      <x:c r="B25" s="0" t="s">
+        <x:v>75</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>